<commit_message>
feat: get ERC721 listing events
</commit_message>
<xml_diff>
--- a/baazaar_sales.xlsx
+++ b/baazaar_sales.xlsx
@@ -959,6 +959,9 @@
       <c r="J21" t="str">
         <v>swap</v>
       </c>
+      <c r="L21" t="str">
+        <v>0xc001874e440d76f77297fa9b5fc3dbb9c0b947095de7ec19251180b9e187b45f</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -985,6 +988,9 @@
       <c r="J22" t="str">
         <v>swap</v>
       </c>
+      <c r="L22" t="str">
+        <v>0xf028a95e6ca63d28a45fca7c293e15431e2cda03a696009f35d5fe3f99b3ec34</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1011,6 +1017,9 @@
       <c r="J23" t="str">
         <v>swap</v>
       </c>
+      <c r="L23" t="str">
+        <v>0x135b23240803be669a729043d04e2a8cbc8c8333f1d06dabcec296433a958b97</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1037,6 +1046,9 @@
       <c r="J24" t="str">
         <v>swap</v>
       </c>
+      <c r="L24" t="str">
+        <v>0xb4e680693a96abe28ce43ab3870d04603e7aaca1e0e3bc45f64a22db30a95f94</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1063,6 +1075,9 @@
       <c r="J25" t="str">
         <v>swap</v>
       </c>
+      <c r="L25" t="str">
+        <v>0x965a1c3653b64f1314ceb7b679d84c6c4abdb039f6412c622740ed4453daa350</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1089,6 +1104,9 @@
       <c r="J26" t="str">
         <v>swap</v>
       </c>
+      <c r="L26" t="str">
+        <v>0xa10aa475db232ba858b40fbf4bb112f159c3a987c82ce5dbc23375147b2f4970</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1115,6 +1133,9 @@
       <c r="J27" t="str">
         <v>swap</v>
       </c>
+      <c r="L27" t="str">
+        <v>0xcba5c4307728b97b52ccbb0202318b2ae3830bad56f9874c955927fa7d0e24e9</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1193,6 +1214,9 @@
       <c r="J30" t="str">
         <v>swap</v>
       </c>
+      <c r="L30" t="str">
+        <v>0xe46aef57ab1277742cdb4615b445f84daa3d9c70167b408421afd483bef6b332</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1219,6 +1243,9 @@
       <c r="J31" t="str">
         <v>swap</v>
       </c>
+      <c r="L31" t="str">
+        <v>0x2900626516b016991b364d256a73dd9eb06fcbc936322ccfee69f9cb02408933</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1245,6 +1272,9 @@
       <c r="J32" t="str">
         <v>swap</v>
       </c>
+      <c r="L32" t="str">
+        <v>0x252f9446583fe02212b888e28cb3ab45564296b837c0a485d629c825380299a8</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1271,6 +1301,9 @@
       <c r="J33" t="str">
         <v>swap</v>
       </c>
+      <c r="L33" t="str">
+        <v>0x75d18e16e30be2eac97853b25325577de49c3102e14a200501a454b371b1eced</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1375,6 +1408,9 @@
       <c r="J37" t="str">
         <v>swap</v>
       </c>
+      <c r="L37" t="str">
+        <v>0x833c30b44bf502ca6f8d1fe3656bee1baee94d00fabbce187d2385c5b5164f8a</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1531,6 +1567,9 @@
       <c r="J43" t="str">
         <v>swap</v>
       </c>
+      <c r="L43" t="str">
+        <v>0xb2951b4893486cdec69fac7d58463cbed0e259ce11dc63f3fa60de30c919995c</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1661,6 +1700,9 @@
       <c r="J48" t="str">
         <v>swap</v>
       </c>
+      <c r="L48" t="str">
+        <v>0xdd0ea5ce8ca55b47eaf710662ee13eb4c02117fd7a7dc86218681f567ce885e0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1687,6 +1729,9 @@
       <c r="J49" t="str">
         <v>swap</v>
       </c>
+      <c r="L49" t="str">
+        <v>0x3022d7ba3378fcf3761e94ce5aa595327010f241902489e5e77d3b06fa7e7e64</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1713,6 +1758,9 @@
       <c r="J50" t="str">
         <v>swap</v>
       </c>
+      <c r="L50" t="str">
+        <v>0xa30e02309b9c7ecc01c9059aef8e849dcd6ee37cd7d42ae6571af399553efee7</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1765,6 +1813,9 @@
       <c r="J52" t="str">
         <v>swap</v>
       </c>
+      <c r="L52" t="str">
+        <v>0x3777721d0a0367cc4ef054fad4b504923472cd18f799e74c132bb2451aeed4a9</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1791,6 +1842,9 @@
       <c r="J53" t="str">
         <v>swap</v>
       </c>
+      <c r="L53" t="str">
+        <v>0x248ea178da7022cdcda30a4458a7a7508c7800ead3833bd6b6c0f759dc84167d</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1817,6 +1871,9 @@
       <c r="J54" t="str">
         <v>swap</v>
       </c>
+      <c r="L54" t="str">
+        <v>0x5a895ea59a5bff39a0d62f2fa02bd32db177562974c15493fa0186d88fb363c2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1843,6 +1900,9 @@
       <c r="J55" t="str">
         <v>swap</v>
       </c>
+      <c r="L55" t="str">
+        <v>0x92e55023eb0ef69cc3fd43c3c669b786daa2f4e4cbdf0699ef3e508f4e455533</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1869,6 +1929,9 @@
       <c r="J56" t="str">
         <v>swap</v>
       </c>
+      <c r="L56" t="str">
+        <v>0x968cccb0cb33c16d88475de655d43af79a35b0cec88ac6ad820c44eb67d1015c</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1895,6 +1958,9 @@
       <c r="J57" t="str">
         <v>swap</v>
       </c>
+      <c r="L57" t="str">
+        <v>0xff11d39511df28f8cd74de6f63215282af0c8b6a1bcdb86d7bed437c62eca38a</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1921,6 +1987,9 @@
       <c r="J58" t="str">
         <v>swap</v>
       </c>
+      <c r="L58" t="str">
+        <v>0xc808dea1de1ca80a346113521e8eee23e1ee504f50c2ff4a3300ec4c70d4b6c2</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1947,6 +2016,9 @@
       <c r="J59" t="str">
         <v>swap</v>
       </c>
+      <c r="L59" t="str">
+        <v>0x6d8462c0d8d216414877b54e9ba7dad2f9519e18d8070b1b2c10b23d5e550dae</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1973,6 +2045,9 @@
       <c r="J60" t="str">
         <v>swap</v>
       </c>
+      <c r="L60" t="str">
+        <v>0xf8b500320e2f3c7cc56aeeac8a6e162c68f5f0434e190605e108c7e970028ae8</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1999,6 +2074,9 @@
       <c r="J61" t="str">
         <v>swap</v>
       </c>
+      <c r="L61" t="str">
+        <v>0x6eee60083c0e375a40bcb46aabe2027a93e2eac01d99a38d293872abd020f3e6</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -2025,6 +2103,9 @@
       <c r="J62" t="str">
         <v>swap</v>
       </c>
+      <c r="L62" t="str">
+        <v>0x6fde78f16413e8d7164c99a5d4c00ffd5cb2410f4983fba696e3e3f9eb6d66e3</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -2051,6 +2132,9 @@
       <c r="J63" t="str">
         <v>swap</v>
       </c>
+      <c r="L63" t="str">
+        <v>0x771ce0823d559f266e9d5bc590510b47da83232804f5d2d7404ba89394bb2a59</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -2077,6 +2161,9 @@
       <c r="J64" t="str">
         <v>swap</v>
       </c>
+      <c r="L64" t="str">
+        <v>0x6b6b3eaa0dd39229f7add81aa1467b80453b9dcfbc17a9c3d541682950114d5c</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -2103,6 +2190,9 @@
       <c r="J65" t="str">
         <v>swap</v>
       </c>
+      <c r="L65" t="str">
+        <v>0xb8fe37e67bbf0f8f52f83d149a7feb5d2dad8a555cef3d6950cb989f944e5cb4</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -2129,6 +2219,9 @@
       <c r="J66" t="str">
         <v>swap</v>
       </c>
+      <c r="L66" t="str">
+        <v>0xe03333eb0e8844ce9997af941a1cdaadcc0404bea48ee94a6a5484b645b2628a</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -2155,6 +2248,9 @@
       <c r="J67" t="str">
         <v>swap</v>
       </c>
+      <c r="L67" t="str">
+        <v>0x09a4561fbda51f6f1d26bbccbd667eb9237a8cf00dd3af7e9e3ee3615ae83d3c</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -2181,6 +2277,9 @@
       <c r="J68" t="str">
         <v>swap</v>
       </c>
+      <c r="L68" t="str">
+        <v>0x1321559efdb06cf82ed098bf1847a73ca706c853e0e0afb05a44c7b81fac930a</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -2207,6 +2306,9 @@
       <c r="J69" t="str">
         <v>swap</v>
       </c>
+      <c r="L69" t="str">
+        <v>0xb22c77d7241cf858bf09c09a3a4b269ec06660f0ee3a7c063be5118b63dfd71a</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -2233,6 +2335,9 @@
       <c r="J70" t="str">
         <v>swap</v>
       </c>
+      <c r="L70" t="str">
+        <v>0x7de46b820ba288c188c5a419f1d761a9d1fdb5a9fc78a7d7419a5f2d5b9e76ca</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -2337,6 +2442,9 @@
       <c r="J74" t="str">
         <v>swap</v>
       </c>
+      <c r="L74" t="str">
+        <v>0xcd320730312cee012376ec831ecfff9a14cdda6267756f9f15549c5514ac48ce</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -2363,6 +2471,9 @@
       <c r="J75" t="str">
         <v>swap</v>
       </c>
+      <c r="L75" t="str">
+        <v>0xb88e49974790e4dd7d4fb5fd8c87d90f0361734c86b27b11a4a125370dea909e</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -2389,6 +2500,9 @@
       <c r="J76" t="str">
         <v>swap</v>
       </c>
+      <c r="L76" t="str">
+        <v>0x2f8784f31432dab15d6051eb0f2a548e9c7789d2e1efd6ec3c567a1d22731978</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -2415,6 +2529,9 @@
       <c r="J77" t="str">
         <v>swap</v>
       </c>
+      <c r="L77" t="str">
+        <v>0x4a5933eec7afca5f190ca463a5add8dfc4a7945b726b8662f210e18dc9b769c6</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -2441,6 +2558,9 @@
       <c r="J78" t="str">
         <v>swap</v>
       </c>
+      <c r="L78" t="str">
+        <v>0x8d79f25da6c0ea5e26a8d326361ad13a63dbe140c8711aa12ccd38bcdfc4253e</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -2467,6 +2587,9 @@
       <c r="J79" t="str">
         <v>swap</v>
       </c>
+      <c r="L79" t="str">
+        <v>0x74f60c474411fd9df085256deb3242a824f17f141b6341da08374142df669b60</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -2493,6 +2616,9 @@
       <c r="J80" t="str">
         <v>swap</v>
       </c>
+      <c r="L80" t="str">
+        <v>0x648d1c9fbd59a3e0f1f5f22b8c693117d42bfeae6a4d90fd1bbda2e608e3715f</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -2519,6 +2645,9 @@
       <c r="J81" t="str">
         <v>swap</v>
       </c>
+      <c r="L81" t="str">
+        <v>0xea2abe76de1a7eb5615377440678d88d271f53239802f480182a0857511fe876</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -2545,6 +2674,9 @@
       <c r="J82" t="str">
         <v>swap</v>
       </c>
+      <c r="L82" t="str">
+        <v>0x9d30d137c8a641897bd9bddc142e135b790b4b7e4997dcff3f1224c2c0d7f4f3</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -2571,6 +2703,9 @@
       <c r="J83" t="str">
         <v>swap</v>
       </c>
+      <c r="L83" t="str">
+        <v>0xd5694aeb24ca8a2a5d03fe24724f3c5edbe61ab319f1323b95c511b178bdfffd</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -2713,6 +2848,9 @@
       <c r="J88" t="str">
         <v>swap</v>
       </c>
+      <c r="L88" t="str">
+        <v>0xe7e93f3bad3d4506e3d0d582891946a73e703a1a81b243bd50b66d7c355e605c</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -2796,6 +2934,9 @@
       </c>
       <c r="J91" t="str">
         <v>swap</v>
+      </c>
+      <c r="L91" t="str">
+        <v>0x748000d006c49e4861cef2aff6c72145f141d6e77b797bb9f6587b4780a76019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: get GBM realm bids
</commit_message>
<xml_diff>
--- a/baazaar_sales.xlsx
+++ b/baazaar_sales.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -465,6 +465,9 @@
       <c r="J2" t="str">
         <v>swap</v>
       </c>
+      <c r="L2" t="str">
+        <v>0xcf51dc81a7306ebf672445bde475d1707846d0337ced6dd782b8523195a8c2ba</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -491,6 +494,9 @@
       <c r="J3" t="str">
         <v>swap</v>
       </c>
+      <c r="L3" t="str">
+        <v>0xcb59a17d02bc17d57a48db04e67d56447987d82aeab1cf111d894a41bb6b1083</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -517,6 +523,9 @@
       <c r="J4" t="str">
         <v>swap</v>
       </c>
+      <c r="L4" t="str">
+        <v>0x8a88687020ac208b642dc608845bf5bfcb48acbd8433822a5659433eb3e5dfa2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -543,6 +552,9 @@
       <c r="J5" t="str">
         <v>swap</v>
       </c>
+      <c r="L5" t="str">
+        <v>0xd537609a6c900c6fdd7f76f6f9490c82708c9a82570a5a6d5330b01a473e6b6e</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -569,6 +581,9 @@
       <c r="J6" t="str">
         <v>swap</v>
       </c>
+      <c r="L6" t="str">
+        <v>0x174fb85943e0afa319b82e02c29a4a3b28ed992f8e197e58b5d80e314ef94b50</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -595,6 +610,9 @@
       <c r="J7" t="str">
         <v>swap</v>
       </c>
+      <c r="L7" t="str">
+        <v>0x07821606d3fecf43c08545100ecbf31ec58cb316baffb3be4c184811788b8196</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -621,6 +639,9 @@
       <c r="J8" t="str">
         <v>swap</v>
       </c>
+      <c r="L8" t="str">
+        <v>0x09b192ecdac332d531c14e1e709173f15d203fd615fa665c32a58d79bf434cf3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -647,6 +668,9 @@
       <c r="J9" t="str">
         <v>swap</v>
       </c>
+      <c r="L9" t="str">
+        <v>0x84fd8e251f6a8244f2375e55391e62732b68fc42aed8000ac9754e2cc787cfda</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -673,6 +697,9 @@
       <c r="J10" t="str">
         <v>swap</v>
       </c>
+      <c r="L10" t="str">
+        <v>0xec3aed6088347695ae0b0877d5fdbf651a05f0ff6127542053713bbe57c4ce50</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -699,6 +726,9 @@
       <c r="J11" t="str">
         <v>swap</v>
       </c>
+      <c r="L11" t="str">
+        <v>0x4b13c4ff5f5d8e695d515a7aeecfd59ff118c86df71f990eeaf1a07aba2000ad</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -725,6 +755,9 @@
       <c r="J12" t="str">
         <v>swap</v>
       </c>
+      <c r="L12" t="str">
+        <v>0x43d569c57f1b0c2f93205d7a42187115541c9efe86d9baff867f9e6bdd1b2446</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -751,6 +784,9 @@
       <c r="J13" t="str">
         <v>swap</v>
       </c>
+      <c r="L13" t="str">
+        <v>0x89045663cbf8e7b581fc7396bb8c8a4ca64f9d72d7dd2d667876b2a99c872eeb</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -777,6 +813,9 @@
       <c r="J14" t="str">
         <v>swap</v>
       </c>
+      <c r="L14" t="str">
+        <v>0xf60fc797a69196e21f1f8d5df79a81deaa93a233d039597bcd64c01c005d9ebc</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -803,6 +842,9 @@
       <c r="J15" t="str">
         <v>swap</v>
       </c>
+      <c r="L15" t="str">
+        <v>0x3fbc8a48c10c0e0da4d84174e79ef9710f0adec3164451cc628437fd1e8b8eec</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -829,6 +871,9 @@
       <c r="J16" t="str">
         <v>swap</v>
       </c>
+      <c r="L16" t="str">
+        <v>0xa830eb6ba411b2b0c55ec77a1ab70843ef145ac1bdd163312c11a88339a3fc6c</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -855,6 +900,9 @@
       <c r="J17" t="str">
         <v>swap</v>
       </c>
+      <c r="L17" t="str">
+        <v>0x08faf95063087647db116a3eab0661253f404e3e5f803e5136e0a679229e8ec2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -881,6 +929,9 @@
       <c r="J18" t="str">
         <v>swap</v>
       </c>
+      <c r="L18" t="str">
+        <v>0xdd5b6b59722acf989347d3de59cd06fc52197d210c923483c261e65cbb1e748a</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -907,22 +958,25 @@
       <c r="J19" t="str">
         <v>swap</v>
       </c>
+      <c r="L19" t="str">
+        <v>0x88e843a8d2226607ce685260a6eea1cfef6c4d19a3460dca2a64ac98273252ac</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2021-11-01 10:59:49 UTC</v>
+        <v>2021-12-02 22:57:43 UTC</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>407</v>
       </c>
       <c r="C20" t="str">
-        <v>GOTCHI ERC1155 #6</v>
+        <v>GHST</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E20" t="str">
-        <v>GHST</v>
+        <v>REALM ERC721 #7816</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -936,19 +990,19 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2021-09-01 16:48:16 UTC</v>
+        <v>2021-11-01 10:59:49 UTC</v>
       </c>
       <c r="B21">
-        <v>999</v>
+        <v>5</v>
       </c>
       <c r="C21" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #6</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E21" t="str">
-        <v>GOTCHI ERC721 #19688</v>
+        <v>GHST</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -960,24 +1014,24 @@
         <v>swap</v>
       </c>
       <c r="L21" t="str">
-        <v>0xc001874e440d76f77297fa9b5fc3dbb9c0b947095de7ec19251180b9e187b45f</v>
+        <v>0x9ce2c2e4fd709f8db8365f4ecb3bf0f4c2eb271c805f53f28ea3659cf00bed56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>2021-08-31 22:57:01 UTC</v>
+        <v>2021-10-31 13:00:31 UTC</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>332.75</v>
       </c>
       <c r="C22" t="str">
-        <v>GOTCHI ERC721 #20615</v>
+        <v>GHST</v>
       </c>
       <c r="D22">
-        <v>310</v>
+        <v>1</v>
       </c>
       <c r="E22" t="str">
-        <v>GHST</v>
+        <v>REALM ERC721 #19107</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -987,17 +1041,14 @@
       </c>
       <c r="J22" t="str">
         <v>swap</v>
-      </c>
-      <c r="L22" t="str">
-        <v>0xf028a95e6ca63d28a45fca7c293e15431e2cda03a696009f35d5fe3f99b3ec34</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>2021-08-31 16:54:44 UTC</v>
+        <v>2021-09-01 16:48:16 UTC</v>
       </c>
       <c r="B23">
-        <v>248</v>
+        <v>999</v>
       </c>
       <c r="C23" t="str">
         <v>GHST</v>
@@ -1006,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="str">
-        <v>GOTCHI ERC721 #20615</v>
+        <v>GOTCHI ERC721 #19688</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1018,21 +1069,21 @@
         <v>swap</v>
       </c>
       <c r="L23" t="str">
-        <v>0x135b23240803be669a729043d04e2a8cbc8c8333f1d06dabcec296433a958b97</v>
+        <v>0xc001874e440d76f77297fa9b5fc3dbb9c0b947095de7ec19251180b9e187b45f</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>2021-08-30 11:47:24 UTC</v>
+        <v>2021-08-31 22:57:01 UTC</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="str">
-        <v>GOTCHI ERC1155 #242</v>
+        <v>GOTCHI ERC721 #20615</v>
       </c>
       <c r="D24">
-        <v>400</v>
+        <v>310</v>
       </c>
       <c r="E24" t="str">
         <v>GHST</v>
@@ -1047,24 +1098,24 @@
         <v>swap</v>
       </c>
       <c r="L24" t="str">
-        <v>0xb4e680693a96abe28ce43ab3870d04603e7aaca1e0e3bc45f64a22db30a95f94</v>
+        <v>0xf028a95e6ca63d28a45fca7c293e15431e2cda03a696009f35d5fe3f99b3ec34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>2021-08-11 17:58:11 UTC</v>
+        <v>2021-08-31 16:54:44 UTC</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>248</v>
       </c>
       <c r="C25" t="str">
-        <v>GOTCHI ERC721 #1079</v>
+        <v>GHST</v>
       </c>
       <c r="D25">
-        <v>1050</v>
+        <v>1</v>
       </c>
       <c r="E25" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC721 #20615</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1076,21 +1127,21 @@
         <v>swap</v>
       </c>
       <c r="L25" t="str">
-        <v>0x965a1c3653b64f1314ceb7b679d84c6c4abdb039f6412c622740ed4453daa350</v>
+        <v>0x135b23240803be669a729043d04e2a8cbc8c8333f1d06dabcec296433a958b97</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>2021-08-06 17:18:44 UTC</v>
+        <v>2021-08-30 11:47:24 UTC</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="str">
-        <v>GOTCHI ERC1155 #146</v>
+        <v>GOTCHI ERC1155 #242</v>
       </c>
       <c r="D26">
-        <v>34</v>
+        <v>400</v>
       </c>
       <c r="E26" t="str">
         <v>GHST</v>
@@ -1105,24 +1156,24 @@
         <v>swap</v>
       </c>
       <c r="L26" t="str">
-        <v>0xa10aa475db232ba858b40fbf4bb112f159c3a987c82ce5dbc23375147b2f4970</v>
+        <v>0xb4e680693a96abe28ce43ab3870d04603e7aaca1e0e3bc45f64a22db30a95f94</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>2021-08-05 15:52:10 UTC</v>
+        <v>2021-08-11 17:58:11 UTC</v>
       </c>
       <c r="B27">
-        <v>708.652551</v>
+        <v>1</v>
       </c>
       <c r="C27" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC721 #1079</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>1050</v>
       </c>
       <c r="E27" t="str">
-        <v>GOTCHI ERC721 #1079</v>
+        <v>GHST</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1134,24 +1185,24 @@
         <v>swap</v>
       </c>
       <c r="L27" t="str">
-        <v>0xcba5c4307728b97b52ccbb0202318b2ae3830bad56f9874c955927fa7d0e24e9</v>
+        <v>0x965a1c3653b64f1314ceb7b679d84c6c4abdb039f6412c622740ed4453daa350</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>2021-08-05 15:52:10 UTC</v>
+        <v>2021-08-06 17:18:44 UTC</v>
       </c>
       <c r="B28">
-        <v>11.599549</v>
+        <v>1</v>
       </c>
       <c r="C28" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #146</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E28" t="str">
-        <v>GOTCHI ERC1155 #137</v>
+        <v>GHST</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1161,6 +1212,9 @@
       </c>
       <c r="J28" t="str">
         <v>swap</v>
+      </c>
+      <c r="L28" t="str">
+        <v>0xa10aa475db232ba858b40fbf4bb112f159c3a987c82ce5dbc23375147b2f4970</v>
       </c>
     </row>
     <row r="29">
@@ -1168,7 +1222,7 @@
         <v>2021-08-05 15:52:10 UTC</v>
       </c>
       <c r="B29">
-        <v>64.74789999999997</v>
+        <v>708.652551</v>
       </c>
       <c r="C29" t="str">
         <v>GHST</v>
@@ -1177,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="str">
-        <v>GOTCHI ERC1155 #146</v>
+        <v>GOTCHI ERC721 #1079</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1187,23 +1241,26 @@
       </c>
       <c r="J29" t="str">
         <v>swap</v>
+      </c>
+      <c r="L29" t="str">
+        <v>0xcba5c4307728b97b52ccbb0202318b2ae3830bad56f9874c955927fa7d0e24e9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>2021-07-26 22:56:25 UTC</v>
+        <v>2021-08-05 15:52:10 UTC</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>11.599549</v>
       </c>
       <c r="C30" t="str">
-        <v>GOTCHI ERC1155 #96</v>
+        <v>GHST</v>
       </c>
       <c r="D30">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="E30" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #137</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1213,26 +1270,23 @@
       </c>
       <c r="J30" t="str">
         <v>swap</v>
-      </c>
-      <c r="L30" t="str">
-        <v>0xe46aef57ab1277742cdb4615b445f84daa3d9c70167b408421afd483bef6b332</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>2021-07-24 05:09:25 UTC</v>
+        <v>2021-08-05 15:52:10 UTC</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>64.74789999999997</v>
       </c>
       <c r="C31" t="str">
-        <v>GOTCHI ERC721 #6475</v>
+        <v>GHST</v>
       </c>
       <c r="D31">
-        <v>1050</v>
+        <v>1</v>
       </c>
       <c r="E31" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #146</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1242,23 +1296,20 @@
       </c>
       <c r="J31" t="str">
         <v>swap</v>
-      </c>
-      <c r="L31" t="str">
-        <v>0x2900626516b016991b364d256a73dd9eb06fcbc936322ccfee69f9cb02408933</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>2021-07-24 01:00:29 UTC</v>
+        <v>2021-07-26 22:56:25 UTC</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="str">
-        <v>GOTCHI ERC1155 #21</v>
+        <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="D32">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="E32" t="str">
         <v>GHST</v>
@@ -1273,21 +1324,21 @@
         <v>swap</v>
       </c>
       <c r="L32" t="str">
-        <v>0x252f9446583fe02212b888e28cb3ab45564296b837c0a485d629c825380299a8</v>
+        <v>0xe46aef57ab1277742cdb4615b445f84daa3d9c70167b408421afd483bef6b332</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>2021-07-24 01:00:01 UTC</v>
+        <v>2021-07-24 05:09:25 UTC</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="str">
-        <v>GOTCHI ERC1155 #22</v>
+        <v>GOTCHI ERC721 #6475</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>1050</v>
       </c>
       <c r="E33" t="str">
         <v>GHST</v>
@@ -1302,24 +1353,24 @@
         <v>swap</v>
       </c>
       <c r="L33" t="str">
-        <v>0x75d18e16e30be2eac97853b25325577de49c3102e14a200501a454b371b1eced</v>
+        <v>0x2900626516b016991b364d256a73dd9eb06fcbc936322ccfee69f9cb02408933</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>2021-07-18 09:57:46 UTC</v>
+        <v>2021-07-24 01:00:29 UTC</v>
       </c>
       <c r="B34">
-        <v>12.1</v>
+        <v>1</v>
       </c>
       <c r="C34" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #21</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E34" t="str">
-        <v>GOTCHI ERC1155 #205</v>
+        <v>GHST</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1329,23 +1380,26 @@
       </c>
       <c r="J34" t="str">
         <v>swap</v>
+      </c>
+      <c r="L34" t="str">
+        <v>0x252f9446583fe02212b888e28cb3ab45564296b837c0a485d629c825380299a8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>2021-07-16 16:29:22 UTC</v>
+        <v>2021-07-24 01:00:01 UTC</v>
       </c>
       <c r="B35">
-        <v>169.4</v>
+        <v>1</v>
       </c>
       <c r="C35" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #22</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E35" t="str">
-        <v>GOTCHI ERC1155 #203</v>
+        <v>GHST</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1355,14 +1409,17 @@
       </c>
       <c r="J35" t="str">
         <v>swap</v>
+      </c>
+      <c r="L35" t="str">
+        <v>0x75d18e16e30be2eac97853b25325577de49c3102e14a200501a454b371b1eced</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>2021-07-15 20:24:52 UTC</v>
+        <v>2021-07-18 09:57:46 UTC</v>
       </c>
       <c r="B36">
-        <v>400.4</v>
+        <v>12.1</v>
       </c>
       <c r="C36" t="str">
         <v>GHST</v>
@@ -1371,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="str">
-        <v>GOTCHI ERC1155 #199</v>
+        <v>GOTCHI ERC1155 #205</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1385,10 +1442,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>2021-07-12 10:27:53 UTC</v>
+        <v>2021-07-16 16:29:22 UTC</v>
       </c>
       <c r="B37">
-        <v>919.5590709999999</v>
+        <v>169.4</v>
       </c>
       <c r="C37" t="str">
         <v>GHST</v>
@@ -1397,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="str">
-        <v>GOTCHI ERC721 #8582</v>
+        <v>GOTCHI ERC1155 #203</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1407,17 +1464,14 @@
       </c>
       <c r="J37" t="str">
         <v>swap</v>
-      </c>
-      <c r="L37" t="str">
-        <v>0x833c30b44bf502ca6f8d1fe3656bee1baee94d00fabbce187d2385c5b5164f8a</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>2021-07-12 10:27:53 UTC</v>
+        <v>2021-07-15 20:24:52 UTC</v>
       </c>
       <c r="B38">
-        <v>47.7436</v>
+        <v>400.4</v>
       </c>
       <c r="C38" t="str">
         <v>GHST</v>
@@ -1426,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="str">
-        <v>GOTCHI ERC1155 #151</v>
+        <v>GOTCHI ERC1155 #199</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1443,7 +1497,7 @@
         <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B39">
-        <v>9.300629</v>
+        <v>919.5590709999999</v>
       </c>
       <c r="C39" t="str">
         <v>GHST</v>
@@ -1452,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="str">
-        <v>GOTCHI ERC1155 #137</v>
+        <v>GOTCHI ERC721 #8582</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1462,6 +1516,9 @@
       </c>
       <c r="J39" t="str">
         <v>swap</v>
+      </c>
+      <c r="L39" t="str">
+        <v>0x833c30b44bf502ca6f8d1fe3656bee1baee94d00fabbce187d2385c5b5164f8a</v>
       </c>
     </row>
     <row r="40">
@@ -1469,7 +1526,7 @@
         <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B40">
-        <v>40.28010000000003</v>
+        <v>47.7436</v>
       </c>
       <c r="C40" t="str">
         <v>GHST</v>
@@ -1478,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="str">
-        <v>GOTCHI ERC1155 #21</v>
+        <v>GOTCHI ERC1155 #151</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1495,7 +1552,7 @@
         <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B41">
-        <v>53.622900000000016</v>
+        <v>9.300629</v>
       </c>
       <c r="C41" t="str">
         <v>GHST</v>
@@ -1504,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="str">
-        <v>GOTCHI ERC1155 #146</v>
+        <v>GOTCHI ERC1155 #137</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1521,7 +1578,7 @@
         <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B42">
-        <v>40.49370000000002</v>
+        <v>40.28010000000003</v>
       </c>
       <c r="C42" t="str">
         <v>GHST</v>
@@ -1530,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="str">
-        <v>GOTCHI ERC1155 #22</v>
+        <v>GOTCHI ERC1155 #21</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1544,19 +1601,19 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>2021-06-25 08:29:12 UTC</v>
+        <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>53.622900000000016</v>
       </c>
       <c r="C43" t="str">
-        <v>GOTCHI ERC721 #5507</v>
+        <v>GHST</v>
       </c>
       <c r="D43">
-        <v>1902.406198</v>
+        <v>1</v>
       </c>
       <c r="E43" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #146</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1566,26 +1623,23 @@
       </c>
       <c r="J43" t="str">
         <v>swap</v>
-      </c>
-      <c r="L43" t="str">
-        <v>0xb2951b4893486cdec69fac7d58463cbed0e259ce11dc63f3fa60de30c919995c</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>2021-06-25 08:29:12 UTC</v>
+        <v>2021-07-12 10:27:53 UTC</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>40.49370000000002</v>
       </c>
       <c r="C44" t="str">
-        <v>GOTCHI ERC1155 #134</v>
+        <v>GHST</v>
       </c>
       <c r="D44">
-        <v>7.588199</v>
+        <v>1</v>
       </c>
       <c r="E44" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #22</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1605,10 +1659,10 @@
         <v>1</v>
       </c>
       <c r="C45" t="str">
-        <v>GOTCHI ERC1155 #136</v>
+        <v>GOTCHI ERC721 #5507</v>
       </c>
       <c r="D45">
-        <v>138.30538800000002</v>
+        <v>1902.406198</v>
       </c>
       <c r="E45" t="str">
         <v>GHST</v>
@@ -1621,6 +1675,9 @@
       </c>
       <c r="J45" t="str">
         <v>swap</v>
+      </c>
+      <c r="L45" t="str">
+        <v>0xb2951b4893486cdec69fac7d58463cbed0e259ce11dc63f3fa60de30c919995c</v>
       </c>
     </row>
     <row r="46">
@@ -1631,10 +1688,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="str">
-        <v>GOTCHI ERC1155 #140</v>
+        <v>GOTCHI ERC1155 #134</v>
       </c>
       <c r="D46">
-        <v>17.466115</v>
+        <v>7.588199</v>
       </c>
       <c r="E46" t="str">
         <v>GHST</v>
@@ -1657,10 +1714,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="str">
-        <v>GOTCHI ERC1155 #135</v>
+        <v>GOTCHI ERC1155 #136</v>
       </c>
       <c r="D47">
-        <v>33.2341</v>
+        <v>138.30538800000002</v>
       </c>
       <c r="E47" t="str">
         <v>GHST</v>
@@ -1677,19 +1734,19 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>2021-06-24 16:21:33 UTC</v>
+        <v>2021-06-25 08:29:12 UTC</v>
       </c>
       <c r="B48">
-        <v>513</v>
+        <v>1</v>
       </c>
       <c r="C48" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #140</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>17.466115</v>
       </c>
       <c r="E48" t="str">
-        <v>GOTCHI ERC721 #2601</v>
+        <v>GHST</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1699,23 +1756,20 @@
       </c>
       <c r="J48" t="str">
         <v>swap</v>
-      </c>
-      <c r="L48" t="str">
-        <v>0xdd0ea5ce8ca55b47eaf710662ee13eb4c02117fd7a7dc86218681f567ce885e0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>2021-06-23 21:42:15 UTC</v>
+        <v>2021-06-25 08:29:12 UTC</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="str">
-        <v>GOTCHI ERC721 #2716</v>
+        <v>GOTCHI ERC1155 #135</v>
       </c>
       <c r="D49">
-        <v>890</v>
+        <v>33.2341</v>
       </c>
       <c r="E49" t="str">
         <v>GHST</v>
@@ -1728,17 +1782,14 @@
       </c>
       <c r="J49" t="str">
         <v>swap</v>
-      </c>
-      <c r="L49" t="str">
-        <v>0x3022d7ba3378fcf3761e94ce5aa595327010f241902489e5e77d3b06fa7e7e64</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>2021-06-23 17:50:29 UTC</v>
+        <v>2021-06-24 16:21:33 UTC</v>
       </c>
       <c r="B50">
-        <v>1060.694612</v>
+        <v>513</v>
       </c>
       <c r="C50" t="str">
         <v>GHST</v>
@@ -1747,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="str">
-        <v>GOTCHI ERC721 #5507</v>
+        <v>GOTCHI ERC721 #2601</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1759,24 +1810,24 @@
         <v>swap</v>
       </c>
       <c r="L50" t="str">
-        <v>0xa30e02309b9c7ecc01c9059aef8e849dcd6ee37cd7d42ae6571af399553efee7</v>
+        <v>0xdd0ea5ce8ca55b47eaf710662ee13eb4c02117fd7a7dc86218681f567ce885e0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>2021-06-23 17:50:29 UTC</v>
+        <v>2021-06-23 21:42:15 UTC</v>
       </c>
       <c r="B51">
-        <v>138.30538800000002</v>
+        <v>1</v>
       </c>
       <c r="C51" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC721 #2716</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>890</v>
       </c>
       <c r="E51" t="str">
-        <v>GOTCHI ERC1155 #136</v>
+        <v>GHST</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1786,14 +1837,17 @@
       </c>
       <c r="J51" t="str">
         <v>swap</v>
+      </c>
+      <c r="L51" t="str">
+        <v>0x3022d7ba3378fcf3761e94ce5aa595327010f241902489e5e77d3b06fa7e7e64</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>2021-06-16 09:31:47 UTC</v>
+        <v>2021-06-23 17:50:29 UTC</v>
       </c>
       <c r="B52">
-        <v>6.9</v>
+        <v>1060.694612</v>
       </c>
       <c r="C52" t="str">
         <v>GHST</v>
@@ -1802,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="str">
-        <v>GOTCHI ERC1155 #90</v>
+        <v>GOTCHI ERC721 #5507</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1814,24 +1868,24 @@
         <v>swap</v>
       </c>
       <c r="L52" t="str">
-        <v>0x3777721d0a0367cc4ef054fad4b504923472cd18f799e74c132bb2451aeed4a9</v>
+        <v>0xa30e02309b9c7ecc01c9059aef8e849dcd6ee37cd7d42ae6571af399553efee7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>2021-04-19 17:54:33 UTC</v>
+        <v>2021-06-23 17:50:29 UTC</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>138.30538800000002</v>
       </c>
       <c r="C53" t="str">
-        <v>GOTCHI ERC1155 #108</v>
+        <v>GHST</v>
       </c>
       <c r="D53">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E53" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #136</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1841,17 +1895,14 @@
       </c>
       <c r="J53" t="str">
         <v>swap</v>
-      </c>
-      <c r="L53" t="str">
-        <v>0x248ea178da7022cdcda30a4458a7a7508c7800ead3833bd6b6c0f759dc84167d</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>2021-04-17 11:32:28 UTC</v>
+        <v>2021-06-16 09:31:47 UTC</v>
       </c>
       <c r="B54">
-        <v>25</v>
+        <v>6.9</v>
       </c>
       <c r="C54" t="str">
         <v>GHST</v>
@@ -1860,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="str">
-        <v>GOTCHI ERC1155 #18</v>
+        <v>GOTCHI ERC1155 #90</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1872,21 +1923,21 @@
         <v>swap</v>
       </c>
       <c r="L54" t="str">
-        <v>0x5a895ea59a5bff39a0d62f2fa02bd32db177562974c15493fa0186d88fb363c2</v>
+        <v>0x3777721d0a0367cc4ef054fad4b504923472cd18f799e74c132bb2451aeed4a9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>2021-04-14 07:24:07 UTC</v>
+        <v>2021-04-19 17:54:33 UTC</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="str">
-        <v>GOTCHI ERC1155 #96</v>
+        <v>GOTCHI ERC1155 #108</v>
       </c>
       <c r="D55">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E55" t="str">
         <v>GHST</v>
@@ -1901,15 +1952,15 @@
         <v>swap</v>
       </c>
       <c r="L55" t="str">
-        <v>0x92e55023eb0ef69cc3fd43c3c669b786daa2f4e4cbdf0699ef3e508f4e455533</v>
+        <v>0x248ea178da7022cdcda30a4458a7a7508c7800ead3833bd6b6c0f759dc84167d</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>2021-04-13 23:49:22 UTC</v>
+        <v>2021-04-17 11:32:28 UTC</v>
       </c>
       <c r="B56">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="C56" t="str">
         <v>GHST</v>
@@ -1918,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="str">
-        <v>GOTCHI ERC1155 #158</v>
+        <v>GOTCHI ERC1155 #18</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1930,24 +1981,24 @@
         <v>swap</v>
       </c>
       <c r="L56" t="str">
-        <v>0x968cccb0cb33c16d88475de655d43af79a35b0cec88ac6ad820c44eb67d1015c</v>
+        <v>0x5a895ea59a5bff39a0d62f2fa02bd32db177562974c15493fa0186d88fb363c2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>2021-04-13 22:29:53 UTC</v>
+        <v>2021-04-14 07:24:07 UTC</v>
       </c>
       <c r="B57">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="C57" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E57" t="str">
-        <v>GOTCHI ERC1155 #132</v>
+        <v>GHST</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -1959,24 +2010,24 @@
         <v>swap</v>
       </c>
       <c r="L57" t="str">
-        <v>0xff11d39511df28f8cd74de6f63215282af0c8b6a1bcdb86d7bed437c62eca38a</v>
+        <v>0x92e55023eb0ef69cc3fd43c3c669b786daa2f4e4cbdf0699ef3e508f4e455533</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>2021-04-13 20:55:48 UTC</v>
+        <v>2021-04-13 23:49:22 UTC</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="C58" t="str">
-        <v>GOTCHI ERC1155 #130</v>
+        <v>GHST</v>
       </c>
       <c r="D58">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E58" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #158</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1988,24 +2039,24 @@
         <v>swap</v>
       </c>
       <c r="L58" t="str">
-        <v>0xc808dea1de1ca80a346113521e8eee23e1ee504f50c2ff4a3300ec4c70d4b6c2</v>
+        <v>0x968cccb0cb33c16d88475de655d43af79a35b0cec88ac6ad820c44eb67d1015c</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>2021-04-13 20:55:44 UTC</v>
+        <v>2021-04-13 22:29:53 UTC</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C59" t="str">
-        <v>GOTCHI ERC1155 #79</v>
+        <v>GHST</v>
       </c>
       <c r="D59">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="E59" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #132</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2017,21 +2068,21 @@
         <v>swap</v>
       </c>
       <c r="L59" t="str">
-        <v>0x6d8462c0d8d216414877b54e9ba7dad2f9519e18d8070b1b2c10b23d5e550dae</v>
+        <v>0xff11d39511df28f8cd74de6f63215282af0c8b6a1bcdb86d7bed437c62eca38a</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>2021-04-13 12:39:34 UTC</v>
+        <v>2021-04-13 20:55:48 UTC</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" t="str">
-        <v>GOTCHI ERC1155 #158</v>
+        <v>GOTCHI ERC1155 #130</v>
       </c>
       <c r="D60">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="E60" t="str">
         <v>GHST</v>
@@ -2046,24 +2097,24 @@
         <v>swap</v>
       </c>
       <c r="L60" t="str">
-        <v>0xf8b500320e2f3c7cc56aeeac8a6e162c68f5f0434e190605e108c7e970028ae8</v>
+        <v>0xc808dea1de1ca80a346113521e8eee23e1ee504f50c2ff4a3300ec4c70d4b6c2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>2021-04-13 11:47:25 UTC</v>
+        <v>2021-04-13 20:55:44 UTC</v>
       </c>
       <c r="B61">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C61" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #79</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="E61" t="str">
-        <v>GOTCHI ERC1155 #130</v>
+        <v>GHST</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -2075,21 +2126,21 @@
         <v>swap</v>
       </c>
       <c r="L61" t="str">
-        <v>0x6eee60083c0e375a40bcb46aabe2027a93e2eac01d99a38d293872abd020f3e6</v>
+        <v>0x6d8462c0d8d216414877b54e9ba7dad2f9519e18d8070b1b2c10b23d5e550dae</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>2021-04-13 06:52:59 UTC</v>
+        <v>2021-04-13 12:39:34 UTC</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="str">
-        <v>GOTCHI ERC1155 #60</v>
+        <v>GOTCHI ERC1155 #158</v>
       </c>
       <c r="D62">
-        <v>9.99</v>
+        <v>109</v>
       </c>
       <c r="E62" t="str">
         <v>GHST</v>
@@ -2104,24 +2155,24 @@
         <v>swap</v>
       </c>
       <c r="L62" t="str">
-        <v>0x6fde78f16413e8d7164c99a5d4c00ffd5cb2410f4983fba696e3e3f9eb6d66e3</v>
+        <v>0xf8b500320e2f3c7cc56aeeac8a6e162c68f5f0434e190605e108c7e970028ae8</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>2021-04-12 21:40:31 UTC</v>
+        <v>2021-04-13 11:47:25 UTC</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C63" t="str">
         <v>GHST</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="str">
-        <v>GOTCHI ERC1155 #158</v>
+        <v>GOTCHI ERC1155 #130</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2133,21 +2184,21 @@
         <v>swap</v>
       </c>
       <c r="L63" t="str">
-        <v>0x771ce0823d559f266e9d5bc590510b47da83232804f5d2d7404ba89394bb2a59</v>
+        <v>0x6eee60083c0e375a40bcb46aabe2027a93e2eac01d99a38d293872abd020f3e6</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>2021-04-12 19:18:15 UTC</v>
+        <v>2021-04-13 06:52:59 UTC</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="str">
-        <v>GOTCHI ERC1155 #110</v>
+        <v>GOTCHI ERC1155 #60</v>
       </c>
       <c r="D64">
-        <v>90</v>
+        <v>9.99</v>
       </c>
       <c r="E64" t="str">
         <v>GHST</v>
@@ -2162,24 +2213,24 @@
         <v>swap</v>
       </c>
       <c r="L64" t="str">
-        <v>0x6b6b3eaa0dd39229f7add81aa1467b80453b9dcfbc17a9c3d541682950114d5c</v>
+        <v>0x6fde78f16413e8d7164c99a5d4c00ffd5cb2410f4983fba696e3e3f9eb6d66e3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>2021-04-12 07:05:35 UTC</v>
+        <v>2021-04-12 21:40:31 UTC</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C65" t="str">
-        <v>GOTCHI ERC1155 #94</v>
+        <v>GHST</v>
       </c>
       <c r="D65">
-        <v>12.5</v>
+        <v>1</v>
       </c>
       <c r="E65" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #158</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -2191,24 +2242,24 @@
         <v>swap</v>
       </c>
       <c r="L65" t="str">
-        <v>0xb8fe37e67bbf0f8f52f83d149a7feb5d2dad8a555cef3d6950cb989f944e5cb4</v>
+        <v>0x771ce0823d559f266e9d5bc590510b47da83232804f5d2d7404ba89394bb2a59</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>2021-04-11 20:07:07 UTC</v>
+        <v>2021-04-12 19:18:15 UTC</v>
       </c>
       <c r="B66">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C66" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #110</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="E66" t="str">
-        <v>GOTCHI ERC1155 #130</v>
+        <v>GHST</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -2220,21 +2271,21 @@
         <v>swap</v>
       </c>
       <c r="L66" t="str">
-        <v>0xe03333eb0e8844ce9997af941a1cdaadcc0404bea48ee94a6a5484b645b2628a</v>
+        <v>0x6b6b3eaa0dd39229f7add81aa1467b80453b9dcfbc17a9c3d541682950114d5c</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>2021-04-11 19:46:31 UTC</v>
+        <v>2021-04-12 07:05:35 UTC</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="str">
-        <v>GOTCHI ERC1155 #18</v>
+        <v>GOTCHI ERC1155 #94</v>
       </c>
       <c r="D67">
-        <v>26</v>
+        <v>12.5</v>
       </c>
       <c r="E67" t="str">
         <v>GHST</v>
@@ -2249,15 +2300,15 @@
         <v>swap</v>
       </c>
       <c r="L67" t="str">
-        <v>0x09a4561fbda51f6f1d26bbccbd667eb9237a8cf00dd3af7e9e3ee3615ae83d3c</v>
+        <v>0xb8fe37e67bbf0f8f52f83d149a7feb5d2dad8a555cef3d6950cb989f944e5cb4</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>2021-04-11 19:13:14 UTC</v>
+        <v>2021-04-11 20:07:07 UTC</v>
       </c>
       <c r="B68">
-        <v>325</v>
+        <v>12</v>
       </c>
       <c r="C68" t="str">
         <v>GHST</v>
@@ -2266,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="E68" t="str">
-        <v>GOTCHI ERC1155 #133</v>
+        <v>GOTCHI ERC1155 #130</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2278,24 +2329,24 @@
         <v>swap</v>
       </c>
       <c r="L68" t="str">
-        <v>0x1321559efdb06cf82ed098bf1847a73ca706c853e0e0afb05a44c7b81fac930a</v>
+        <v>0xe03333eb0e8844ce9997af941a1cdaadcc0404bea48ee94a6a5484b645b2628a</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>2021-04-11 13:47:28 UTC</v>
+        <v>2021-04-11 19:46:31 UTC</v>
       </c>
       <c r="B69">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C69" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #18</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E69" t="str">
-        <v>GOTCHI ERC1155 #18</v>
+        <v>GHST</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2307,15 +2358,15 @@
         <v>swap</v>
       </c>
       <c r="L69" t="str">
-        <v>0xb22c77d7241cf858bf09c09a3a4b269ec06660f0ee3a7c063be5118b63dfd71a</v>
+        <v>0x09a4561fbda51f6f1d26bbccbd667eb9237a8cf00dd3af7e9e3ee3615ae83d3c</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>2021-04-10 11:16:52 UTC</v>
+        <v>2021-04-11 19:13:14 UTC</v>
       </c>
       <c r="B70">
-        <v>427.61760000000004</v>
+        <v>325</v>
       </c>
       <c r="C70" t="str">
         <v>GHST</v>
@@ -2324,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="E70" t="str">
-        <v>GOTCHI ERC721 #6475</v>
+        <v>GOTCHI ERC1155 #133</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2336,15 +2387,15 @@
         <v>swap</v>
       </c>
       <c r="L70" t="str">
-        <v>0x7de46b820ba288c188c5a419f1d761a9d1fdb5a9fc78a7d7419a5f2d5b9e76ca</v>
+        <v>0x1321559efdb06cf82ed098bf1847a73ca706c853e0e0afb05a44c7b81fac930a</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>2021-04-10 11:16:52 UTC</v>
+        <v>2021-04-11 13:47:28 UTC</v>
       </c>
       <c r="B71">
-        <v>296.47929999999997</v>
+        <v>20</v>
       </c>
       <c r="C71" t="str">
         <v>GHST</v>
@@ -2353,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="E71" t="str">
-        <v>GOTCHI ERC1155 #79</v>
+        <v>GOTCHI ERC1155 #18</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2363,6 +2414,9 @@
       </c>
       <c r="J71" t="str">
         <v>swap</v>
+      </c>
+      <c r="L71" t="str">
+        <v>0xb22c77d7241cf858bf09c09a3a4b269ec06660f0ee3a7c063be5118b63dfd71a</v>
       </c>
     </row>
     <row r="72">
@@ -2370,7 +2424,7 @@
         <v>2021-04-10 11:16:52 UTC</v>
       </c>
       <c r="B72">
-        <v>49.458899999999964</v>
+        <v>427.61760000000004</v>
       </c>
       <c r="C72" t="str">
         <v>GHST</v>
@@ -2379,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="str">
-        <v>GOTCHI ERC1155 #96</v>
+        <v>GOTCHI ERC721 #6475</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -2389,6 +2443,9 @@
       </c>
       <c r="J72" t="str">
         <v>swap</v>
+      </c>
+      <c r="L72" t="str">
+        <v>0x7de46b820ba288c188c5a419f1d761a9d1fdb5a9fc78a7d7419a5f2d5b9e76ca</v>
       </c>
     </row>
     <row r="73">
@@ -2396,7 +2453,7 @@
         <v>2021-04-10 11:16:52 UTC</v>
       </c>
       <c r="B73">
-        <v>16.444200000000006</v>
+        <v>296.47929999999997</v>
       </c>
       <c r="C73" t="str">
         <v>GHST</v>
@@ -2405,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="E73" t="str">
-        <v>GOTCHI ERC1155 #60</v>
+        <v>GOTCHI ERC1155 #79</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -2419,10 +2476,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>2021-04-09 16:43:51 UTC</v>
+        <v>2021-04-10 11:16:52 UTC</v>
       </c>
       <c r="B74">
-        <v>6</v>
+        <v>49.458899999999964</v>
       </c>
       <c r="C74" t="str">
         <v>GHST</v>
@@ -2431,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="E74" t="str">
-        <v>GOTCHI ERC1155 #134</v>
+        <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -2441,17 +2498,14 @@
       </c>
       <c r="J74" t="str">
         <v>swap</v>
-      </c>
-      <c r="L74" t="str">
-        <v>0xcd320730312cee012376ec831ecfff9a14cdda6267756f9f15549c5514ac48ce</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>2021-04-09 07:07:59 UTC</v>
+        <v>2021-04-10 11:16:52 UTC</v>
       </c>
       <c r="B75">
-        <v>9</v>
+        <v>16.444200000000006</v>
       </c>
       <c r="C75" t="str">
         <v>GHST</v>
@@ -2460,7 +2514,7 @@
         <v>1</v>
       </c>
       <c r="E75" t="str">
-        <v>GOTCHI ERC1155 #135</v>
+        <v>GOTCHI ERC1155 #60</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -2470,17 +2524,14 @@
       </c>
       <c r="J75" t="str">
         <v>swap</v>
-      </c>
-      <c r="L75" t="str">
-        <v>0xb88e49974790e4dd7d4fb5fd8c87d90f0361734c86b27b11a4a125370dea909e</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>2021-04-08 17:28:09 UTC</v>
+        <v>2021-04-09 16:43:51 UTC</v>
       </c>
       <c r="B76">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C76" t="str">
         <v>GHST</v>
@@ -2489,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="str">
-        <v>GOTCHI ERC1155 #136</v>
+        <v>GOTCHI ERC1155 #134</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -2501,15 +2552,15 @@
         <v>swap</v>
       </c>
       <c r="L76" t="str">
-        <v>0x2f8784f31432dab15d6051eb0f2a548e9c7789d2e1efd6ec3c567a1d22731978</v>
+        <v>0xcd320730312cee012376ec831ecfff9a14cdda6267756f9f15549c5514ac48ce</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>2021-04-02 18:34:03 UTC</v>
+        <v>2021-04-09 07:07:59 UTC</v>
       </c>
       <c r="B77">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C77" t="str">
         <v>GHST</v>
@@ -2518,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="str">
-        <v>GOTCHI ERC1155 #137</v>
+        <v>GOTCHI ERC1155 #135</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -2530,24 +2581,24 @@
         <v>swap</v>
       </c>
       <c r="L77" t="str">
-        <v>0x4a5933eec7afca5f190ca463a5add8dfc4a7945b726b8662f210e18dc9b769c6</v>
+        <v>0xb88e49974790e4dd7d4fb5fd8c87d90f0361734c86b27b11a4a125370dea909e</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>2021-04-02 17:06:49 UTC</v>
+        <v>2021-04-08 17:28:09 UTC</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C78" t="str">
-        <v>GOTCHI ERC1155 #64</v>
+        <v>GHST</v>
       </c>
       <c r="D78">
-        <v>7.99</v>
+        <v>1</v>
       </c>
       <c r="E78" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #136</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -2559,15 +2610,15 @@
         <v>swap</v>
       </c>
       <c r="L78" t="str">
-        <v>0x8d79f25da6c0ea5e26a8d326361ad13a63dbe140c8711aa12ccd38bcdfc4253e</v>
+        <v>0x2f8784f31432dab15d6051eb0f2a548e9c7789d2e1efd6ec3c567a1d22731978</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>2021-04-02 14:32:30 UTC</v>
+        <v>2021-04-02 18:34:03 UTC</v>
       </c>
       <c r="B79">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" t="str">
         <v>GHST</v>
@@ -2576,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="E79" t="str">
-        <v>GOTCHI ERC1155 #109</v>
+        <v>GOTCHI ERC1155 #137</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2588,24 +2639,24 @@
         <v>swap</v>
       </c>
       <c r="L79" t="str">
-        <v>0x74f60c474411fd9df085256deb3242a824f17f141b6341da08374142df669b60</v>
+        <v>0x4a5933eec7afca5f190ca463a5add8dfc4a7945b726b8662f210e18dc9b769c6</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>2021-04-02 14:32:14 UTC</v>
+        <v>2021-04-02 17:06:49 UTC</v>
       </c>
       <c r="B80">
-        <v>9.99</v>
+        <v>1</v>
       </c>
       <c r="C80" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #64</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>7.99</v>
       </c>
       <c r="E80" t="str">
-        <v>GOTCHI ERC1155 #108</v>
+        <v>GHST</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -2617,15 +2668,15 @@
         <v>swap</v>
       </c>
       <c r="L80" t="str">
-        <v>0x648d1c9fbd59a3e0f1f5f22b8c693117d42bfeae6a4d90fd1bbda2e608e3715f</v>
+        <v>0x8d79f25da6c0ea5e26a8d326361ad13a63dbe140c8711aa12ccd38bcdfc4253e</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>2021-04-02 14:31:04 UTC</v>
+        <v>2021-04-02 14:32:30 UTC</v>
       </c>
       <c r="B81">
-        <v>66.99</v>
+        <v>10</v>
       </c>
       <c r="C81" t="str">
         <v>GHST</v>
@@ -2634,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>GOTCHI ERC1155 #110</v>
+        <v>GOTCHI ERC1155 #109</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -2646,15 +2697,15 @@
         <v>swap</v>
       </c>
       <c r="L81" t="str">
-        <v>0xea2abe76de1a7eb5615377440678d88d271f53239802f480182a0857511fe876</v>
+        <v>0x74f60c474411fd9df085256deb3242a824f17f141b6341da08374142df669b60</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>2021-04-01 20:31:30 UTC</v>
+        <v>2021-04-02 14:32:14 UTC</v>
       </c>
       <c r="B82">
-        <v>8</v>
+        <v>9.99</v>
       </c>
       <c r="C82" t="str">
         <v>GHST</v>
@@ -2663,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>GOTCHI ERC1155 #140</v>
+        <v>GOTCHI ERC1155 #108</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -2675,24 +2726,24 @@
         <v>swap</v>
       </c>
       <c r="L82" t="str">
-        <v>0x9d30d137c8a641897bd9bddc142e135b790b4b7e4997dcff3f1224c2c0d7f4f3</v>
+        <v>0x648d1c9fbd59a3e0f1f5f22b8c693117d42bfeae6a4d90fd1bbda2e608e3715f</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>2021-03-26 16:57:08 UTC</v>
+        <v>2021-04-02 14:31:04 UTC</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>66.99</v>
       </c>
       <c r="C83" t="str">
-        <v>GOTCHI ERC1155 #1</v>
+        <v>GHST</v>
       </c>
       <c r="D83">
-        <v>2.94</v>
+        <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #110</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -2704,15 +2755,15 @@
         <v>swap</v>
       </c>
       <c r="L83" t="str">
-        <v>0xd5694aeb24ca8a2a5d03fe24724f3c5edbe61ab319f1323b95c511b178bdfffd</v>
+        <v>0xea2abe76de1a7eb5615377440678d88d271f53239802f480182a0857511fe876</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>2021-03-21 16:11:18 UTC</v>
+        <v>2021-04-01 20:31:30 UTC</v>
       </c>
       <c r="B84">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C84" t="str">
         <v>GHST</v>
@@ -2721,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="E84" t="str">
-        <v>GOTCHI ERC1155 #92</v>
+        <v>GOTCHI ERC1155 #140</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2733,24 +2784,24 @@
         <v>swap</v>
       </c>
       <c r="L84" t="str">
-        <v>0x98d2be8452c483016551f0f91468f6c288601dcec01384713e8f1f8d9ebb4222</v>
+        <v>0x9d30d137c8a641897bd9bddc142e135b790b4b7e4997dcff3f1224c2c0d7f4f3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>2021-03-19 21:20:42 UTC</v>
+        <v>2021-03-26 16:57:08 UTC</v>
       </c>
       <c r="B85">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C85" t="str">
-        <v>GHST</v>
+        <v>GOTCHI ERC1155 #1</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>2.94</v>
       </c>
       <c r="E85" t="str">
-        <v>GOTCHI ERC1155 #96</v>
+        <v>GHST</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -2762,15 +2813,15 @@
         <v>swap</v>
       </c>
       <c r="L85" t="str">
-        <v>0x42ae926ea70f1d348112321cea6b2f3b6c5c9b644b6171ab43f4b50df36e5c51</v>
+        <v>0xd5694aeb24ca8a2a5d03fe24724f3c5edbe61ab319f1323b95c511b178bdfffd</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>2021-03-18 19:46:58 UTC</v>
+        <v>2021-03-21 16:11:18 UTC</v>
       </c>
       <c r="B86">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C86" t="str">
         <v>GHST</v>
@@ -2779,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>GOTCHI ERC1155 #94</v>
+        <v>GOTCHI ERC1155 #92</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -2791,15 +2842,15 @@
         <v>swap</v>
       </c>
       <c r="L86" t="str">
-        <v>0x997ccd0fe566b953fd6379277bf01d553c1805a49a49ffd6c1c3d50f82e1ff7e</v>
+        <v>0x98d2be8452c483016551f0f91468f6c288601dcec01384713e8f1f8d9ebb4222</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>2021-03-18 19:14:46 UTC</v>
+        <v>2021-03-19 21:20:42 UTC</v>
       </c>
       <c r="B87">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C87" t="str">
         <v>GHST</v>
@@ -2808,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>GOTCHI ERC1155 #64</v>
+        <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -2820,15 +2871,15 @@
         <v>swap</v>
       </c>
       <c r="L87" t="str">
-        <v>0x6d7a75db64e2dea6c077007b9493cf3b048197bf1e49ff596f26ddd346d19339</v>
+        <v>0x42ae926ea70f1d348112321cea6b2f3b6c5c9b644b6171ab43f4b50df36e5c51</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>2021-03-18 19:09:06 UTC</v>
+        <v>2021-03-18 19:46:58 UTC</v>
       </c>
       <c r="B88">
-        <v>445</v>
+        <v>19</v>
       </c>
       <c r="C88" t="str">
         <v>GHST</v>
@@ -2837,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>GOTCHI ERC721 #2716</v>
+        <v>GOTCHI ERC1155 #94</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -2849,15 +2900,15 @@
         <v>swap</v>
       </c>
       <c r="L88" t="str">
-        <v>0xe7e93f3bad3d4506e3d0d582891946a73e703a1a81b243bd50b66d7c355e605c</v>
+        <v>0x997ccd0fe566b953fd6379277bf01d553c1805a49a49ffd6c1c3d50f82e1ff7e</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>2021-03-17 23:42:27 UTC</v>
+        <v>2021-03-18 19:14:46 UTC</v>
       </c>
       <c r="B89">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C89" t="str">
         <v>GHST</v>
@@ -2866,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="E89" t="str">
-        <v>GOTCHI ERC1155 #91</v>
+        <v>GOTCHI ERC1155 #64</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -2878,15 +2929,15 @@
         <v>swap</v>
       </c>
       <c r="L89" t="str">
-        <v>0x3cf8694242df0ba2a9275bda8819c2984da60c2a1bf73ceed2b52d709c972180</v>
+        <v>0x6d7a75db64e2dea6c077007b9493cf3b048197bf1e49ff596f26ddd346d19339</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>2021-03-14 16:17:30 UTC</v>
+        <v>2021-03-18 19:09:06 UTC</v>
       </c>
       <c r="B90">
-        <v>17</v>
+        <v>445</v>
       </c>
       <c r="C90" t="str">
         <v>GHST</v>
@@ -2895,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="E90" t="str">
-        <v>GOTCHI ERC1155 #90</v>
+        <v>GOTCHI ERC721 #2716</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -2907,41 +2958,99 @@
         <v>swap</v>
       </c>
       <c r="L90" t="str">
-        <v>0x1fb8619fde23827ddccbe1c4cd0a89ffd36d298dfee4430ad36e04ab712e4abc</v>
+        <v>0xe7e93f3bad3d4506e3d0d582891946a73e703a1a81b243bd50b66d7c355e605c</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
+        <v>2021-03-17 23:42:27 UTC</v>
+      </c>
+      <c r="B91">
+        <v>17</v>
+      </c>
+      <c r="C91" t="str">
+        <v>GHST</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="str">
+        <v>GOTCHI ERC1155 #91</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="str">
+        <v>MATIC</v>
+      </c>
+      <c r="J91" t="str">
+        <v>swap</v>
+      </c>
+      <c r="L91" t="str">
+        <v>0x3cf8694242df0ba2a9275bda8819c2984da60c2a1bf73ceed2b52d709c972180</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>2021-03-14 16:17:30 UTC</v>
+      </c>
+      <c r="B92">
+        <v>17</v>
+      </c>
+      <c r="C92" t="str">
+        <v>GHST</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="str">
+        <v>GOTCHI ERC1155 #90</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="str">
+        <v>MATIC</v>
+      </c>
+      <c r="J92" t="str">
+        <v>swap</v>
+      </c>
+      <c r="L92" t="str">
+        <v>0x1fb8619fde23827ddccbe1c4cd0a89ffd36d298dfee4430ad36e04ab712e4abc</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
         <v>2021-03-06 22:21:52 UTC</v>
       </c>
-      <c r="B91">
+      <c r="B93">
         <v>349</v>
       </c>
-      <c r="C91" t="str">
-        <v>GHST</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-      <c r="E91" t="str">
+      <c r="C93" t="str">
+        <v>GHST</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93" t="str">
         <v>GOTCHI ERC721 #5603</v>
       </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91" t="str">
-        <v>MATIC</v>
-      </c>
-      <c r="J91" t="str">
-        <v>swap</v>
-      </c>
-      <c r="L91" t="str">
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="str">
+        <v>MATIC</v>
+      </c>
+      <c r="J93" t="str">
+        <v>swap</v>
+      </c>
+      <c r="L93" t="str">
         <v>0x748000d006c49e4861cef2aff6c72145f141d6e77b797bb9f6587b4780a76019</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L91"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L93"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Sum after sale fee
</commit_message>
<xml_diff>
--- a/baazaar_sales.xlsx
+++ b/baazaar_sales.xlsx
@@ -451,7 +451,7 @@
         <v>GOTCHI ERC1155 #297</v>
       </c>
       <c r="D2">
-        <v>37</v>
+        <v>35.705</v>
       </c>
       <c r="E2" t="str">
         <v>GHST</v>
@@ -480,7 +480,7 @@
         <v>GOTCHI ERC1155 #296</v>
       </c>
       <c r="D3">
-        <v>97</v>
+        <v>93.605</v>
       </c>
       <c r="E3" t="str">
         <v>GHST</v>
@@ -509,7 +509,7 @@
         <v>GOTCHI ERC1155 #298</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>17.37</v>
       </c>
       <c r="E4" t="str">
         <v>GHST</v>
@@ -538,7 +538,7 @@
         <v>GOTCHI ERC1155 #296</v>
       </c>
       <c r="D5">
-        <v>97</v>
+        <v>93.605</v>
       </c>
       <c r="E5" t="str">
         <v>GHST</v>
@@ -567,7 +567,7 @@
         <v>GOTCHI ERC1155 #293</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <v>18.335</v>
       </c>
       <c r="E6" t="str">
         <v>GHST</v>
@@ -596,7 +596,7 @@
         <v>GOTCHI ERC721 #19688</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>965</v>
       </c>
       <c r="E7" t="str">
         <v>GHST</v>
@@ -625,7 +625,7 @@
         <v>GOTCHI ERC1155 #300</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>23.16</v>
       </c>
       <c r="E8" t="str">
         <v>GHST</v>
@@ -654,7 +654,7 @@
         <v>GOTCHI ERC1155 #90</v>
       </c>
       <c r="D9">
-        <v>23</v>
+        <v>22.195</v>
       </c>
       <c r="E9" t="str">
         <v>GHST</v>
@@ -683,7 +683,7 @@
         <v>GOTCHI ERC1155 #90</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>22.195</v>
       </c>
       <c r="E10" t="str">
         <v>GHST</v>
@@ -741,7 +741,7 @@
         <v>GOTCHI ERC1155 #242</v>
       </c>
       <c r="D12">
-        <v>720</v>
+        <v>694.8</v>
       </c>
       <c r="E12" t="str">
         <v>GHST</v>
@@ -770,7 +770,7 @@
         <v>GOTCHI ERC721 #16913</v>
       </c>
       <c r="D13">
-        <v>580</v>
+        <v>559.6999999999999</v>
       </c>
       <c r="E13" t="str">
         <v>GHST</v>
@@ -799,7 +799,7 @@
         <v>GOTCHI ERC1155 #3</v>
       </c>
       <c r="D14">
-        <v>160</v>
+        <v>154.4</v>
       </c>
       <c r="E14" t="str">
         <v>GHST</v>
@@ -828,7 +828,7 @@
         <v>GOTCHI ERC1155 #146</v>
       </c>
       <c r="D15">
-        <v>78</v>
+        <v>75.27</v>
       </c>
       <c r="E15" t="str">
         <v>GHST</v>
@@ -915,7 +915,7 @@
         <v>GOTCHI ERC1155 #6</v>
       </c>
       <c r="D18">
-        <v>33.51</v>
+        <v>32.337149999999994</v>
       </c>
       <c r="E18" t="str">
         <v>GHST</v>
@@ -944,7 +944,7 @@
         <v>GOTCHI ERC1155 #6</v>
       </c>
       <c r="D19">
-        <v>11.17</v>
+        <v>10.77905</v>
       </c>
       <c r="E19" t="str">
         <v>GHST</v>
@@ -999,7 +999,7 @@
         <v>GOTCHI ERC1155 #6</v>
       </c>
       <c r="D21">
-        <v>80</v>
+        <v>77.2</v>
       </c>
       <c r="E21" t="str">
         <v>GHST</v>
@@ -1083,7 +1083,7 @@
         <v>GOTCHI ERC721 #20615</v>
       </c>
       <c r="D24">
-        <v>310</v>
+        <v>299.15</v>
       </c>
       <c r="E24" t="str">
         <v>GHST</v>
@@ -1141,7 +1141,7 @@
         <v>GOTCHI ERC1155 #242</v>
       </c>
       <c r="D26">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="E26" t="str">
         <v>GHST</v>
@@ -1170,7 +1170,7 @@
         <v>GOTCHI ERC721 #1079</v>
       </c>
       <c r="D27">
-        <v>1050</v>
+        <v>1013.25</v>
       </c>
       <c r="E27" t="str">
         <v>GHST</v>
@@ -1199,7 +1199,7 @@
         <v>GOTCHI ERC1155 #146</v>
       </c>
       <c r="D28">
-        <v>34</v>
+        <v>32.81</v>
       </c>
       <c r="E28" t="str">
         <v>GHST</v>
@@ -1309,7 +1309,7 @@
         <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="D32">
-        <v>54</v>
+        <v>52.11</v>
       </c>
       <c r="E32" t="str">
         <v>GHST</v>
@@ -1338,7 +1338,7 @@
         <v>GOTCHI ERC721 #6475</v>
       </c>
       <c r="D33">
-        <v>1050</v>
+        <v>1013.25</v>
       </c>
       <c r="E33" t="str">
         <v>GHST</v>
@@ -1367,7 +1367,7 @@
         <v>GOTCHI ERC1155 #21</v>
       </c>
       <c r="D34">
-        <v>30</v>
+        <v>28.95</v>
       </c>
       <c r="E34" t="str">
         <v>GHST</v>
@@ -1396,7 +1396,7 @@
         <v>GOTCHI ERC1155 #22</v>
       </c>
       <c r="D35">
-        <v>20</v>
+        <v>19.3</v>
       </c>
       <c r="E35" t="str">
         <v>GHST</v>
@@ -1662,7 +1662,7 @@
         <v>GOTCHI ERC721 #5507</v>
       </c>
       <c r="D45">
-        <v>1902.406198</v>
+        <v>1835.8219810699998</v>
       </c>
       <c r="E45" t="str">
         <v>GHST</v>
@@ -1691,7 +1691,7 @@
         <v>GOTCHI ERC1155 #134</v>
       </c>
       <c r="D46">
-        <v>7.588199</v>
+        <v>7.322612035</v>
       </c>
       <c r="E46" t="str">
         <v>GHST</v>
@@ -1717,7 +1717,7 @@
         <v>GOTCHI ERC1155 #136</v>
       </c>
       <c r="D47">
-        <v>138.30538800000002</v>
+        <v>133.46469942000002</v>
       </c>
       <c r="E47" t="str">
         <v>GHST</v>
@@ -1743,7 +1743,7 @@
         <v>GOTCHI ERC1155 #140</v>
       </c>
       <c r="D48">
-        <v>17.466115</v>
+        <v>16.854800974999996</v>
       </c>
       <c r="E48" t="str">
         <v>GHST</v>
@@ -1769,7 +1769,7 @@
         <v>GOTCHI ERC1155 #135</v>
       </c>
       <c r="D49">
-        <v>33.2341</v>
+        <v>32.0709065</v>
       </c>
       <c r="E49" t="str">
         <v>GHST</v>
@@ -1824,7 +1824,7 @@
         <v>GOTCHI ERC721 #2716</v>
       </c>
       <c r="D51">
-        <v>890</v>
+        <v>858.85</v>
       </c>
       <c r="E51" t="str">
         <v>GHST</v>
@@ -1937,7 +1937,7 @@
         <v>GOTCHI ERC1155 #108</v>
       </c>
       <c r="D55">
-        <v>9</v>
+        <v>8.73</v>
       </c>
       <c r="E55" t="str">
         <v>GHST</v>
@@ -1995,7 +1995,7 @@
         <v>GOTCHI ERC1155 #96</v>
       </c>
       <c r="D57">
-        <v>20</v>
+        <v>19.4</v>
       </c>
       <c r="E57" t="str">
         <v>GHST</v>
@@ -2082,7 +2082,7 @@
         <v>GOTCHI ERC1155 #130</v>
       </c>
       <c r="D60">
-        <v>16</v>
+        <v>15.52</v>
       </c>
       <c r="E60" t="str">
         <v>GHST</v>
@@ -2111,7 +2111,7 @@
         <v>GOTCHI ERC1155 #79</v>
       </c>
       <c r="D61">
-        <v>95</v>
+        <v>92.14999999999999</v>
       </c>
       <c r="E61" t="str">
         <v>GHST</v>
@@ -2140,7 +2140,7 @@
         <v>GOTCHI ERC1155 #158</v>
       </c>
       <c r="D62">
-        <v>109</v>
+        <v>105.73</v>
       </c>
       <c r="E62" t="str">
         <v>GHST</v>
@@ -2198,7 +2198,7 @@
         <v>GOTCHI ERC1155 #60</v>
       </c>
       <c r="D64">
-        <v>9.99</v>
+        <v>9.6903</v>
       </c>
       <c r="E64" t="str">
         <v>GHST</v>
@@ -2256,7 +2256,7 @@
         <v>GOTCHI ERC1155 #110</v>
       </c>
       <c r="D66">
-        <v>90</v>
+        <v>87.3</v>
       </c>
       <c r="E66" t="str">
         <v>GHST</v>
@@ -2285,7 +2285,7 @@
         <v>GOTCHI ERC1155 #94</v>
       </c>
       <c r="D67">
-        <v>12.5</v>
+        <v>12.125</v>
       </c>
       <c r="E67" t="str">
         <v>GHST</v>
@@ -2343,7 +2343,7 @@
         <v>GOTCHI ERC1155 #18</v>
       </c>
       <c r="D69">
-        <v>26</v>
+        <v>25.22</v>
       </c>
       <c r="E69" t="str">
         <v>GHST</v>
@@ -2653,7 +2653,7 @@
         <v>GOTCHI ERC1155 #64</v>
       </c>
       <c r="D80">
-        <v>7.99</v>
+        <v>7.7503</v>
       </c>
       <c r="E80" t="str">
         <v>GHST</v>
@@ -2798,7 +2798,7 @@
         <v>GOTCHI ERC1155 #1</v>
       </c>
       <c r="D85">
-        <v>2.94</v>
+        <v>2.8518</v>
       </c>
       <c r="E85" t="str">
         <v>GHST</v>

</xml_diff>